<commit_message>
update breed prediction fig
</commit_message>
<xml_diff>
--- a/metadata/dataset_sum.xlsx
+++ b/metadata/dataset_sum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingxuan/GitHub/canine_tumor_wes/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8565BB-D4D4-984B-B2F1-08F4896A0E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041F3F3A-F899-3841-9F71-F311211706D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29400" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{8C911715-1879-214C-93AA-41359558607D}"/>
   </bookViews>
@@ -1328,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3586624C-3A3C-3A4F-BE02-FCD2422E18D2}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1776,6 +1776,111 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
+    <row r="13" spans="1:13" ht="44" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="5">
+        <v>11</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="44" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="5">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="44" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="5">
+        <v>829</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1783,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF5FF9E-BB60-774C-891F-D2C85E568BFC}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A13" sqref="A13:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2087,111 +2192,6 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="5">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="5">
-        <v>2020</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="5">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="5">
-        <v>2020</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C15" s="5">
-        <v>829</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="5">
-        <v>2022</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>